<commit_message>
Added seperate test case for validaqting followers count Modified search test validation Modified java compiler to 1.8
</commit_message>
<xml_diff>
--- a/src/test/test-data/FollowTestData.xlsx
+++ b/src/test/test-data/FollowTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="60">
   <si>
     <t>GET</t>
   </si>
@@ -190,7 +190,10 @@
     <t>status=403||followRelationship:IS_NONE</t>
   </si>
   <si>
-    <t>status=200||count=2</t>
+    <t>count</t>
+  </si>
+  <si>
+    <t>S1_TC_T14</t>
   </si>
 </sst>
 </file>
@@ -564,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L14"/>
+      <selection activeCell="L2" sqref="L2:L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -804,46 +807,46 @@
       </c>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" ht="45">
       <c r="A10" t="s">
         <v>47</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="H10"/>
       <c r="J10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30">
       <c r="A11" t="s">
         <v>48</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
         <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="E11" t="s">
         <v>23</v>
       </c>
       <c r="H11"/>
       <c r="J11" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="30">
@@ -851,7 +854,7 @@
         <v>49</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
         <v>21</v>
@@ -864,7 +867,7 @@
       </c>
       <c r="H12"/>
       <c r="J12" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30">
@@ -872,46 +875,74 @@
         <v>52</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
         <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13"/>
+        <v>56</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="1"/>
       <c r="J13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="30">
+        <v>57</v>
+      </c>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>54</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
         <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14"/>
+      <c r="J14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="30">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="1"/>
-      <c r="J14" t="s">
-        <v>57</v>
-      </c>
-      <c r="K14" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="1"/>
+      <c r="J15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added new test cases in 1PFOLLOW Added new test case in 1PAUTH
</commit_message>
<xml_diff>
--- a/src/test/test-data/FollowTestData.xlsx
+++ b/src/test/test-data/FollowTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="93">
   <si>
     <t>GET</t>
   </si>
@@ -194,6 +194,105 @@
   </si>
   <si>
     <t>S1_TC_T14</t>
+  </si>
+  <si>
+    <t>verify follow relationship when the user doesn't follow each other</t>
+  </si>
+  <si>
+    <t>/follow/user/(SYS_USER2)/relations</t>
+  </si>
+  <si>
+    <t>?id=(SYS_USER1)</t>
+  </si>
+  <si>
+    <t>status=200||(SYS_USER1)=IS_NONE</t>
+  </si>
+  <si>
+    <t>verify follow relationship by passing empty key and test error status</t>
+  </si>
+  <si>
+    <t>?id=</t>
+  </si>
+  <si>
+    <t>status=500||errorCode=500||errorMessage=Key may not be empty</t>
+  </si>
+  <si>
+    <t>verify follow relationship when the user follower of other</t>
+  </si>
+  <si>
+    <t>/follow/user/(SYS_USER1)/relations</t>
+  </si>
+  <si>
+    <t>?id=(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>status=200||(SYS_USER2)=IS_FOLLOWER</t>
+  </si>
+  <si>
+    <t>status=200||(SYS_USER1)=IS_FOLLOWED</t>
+  </si>
+  <si>
+    <t>Get all followers information</t>
+  </si>
+  <si>
+    <t>/follow/user/(SYS_USER1)/followers/profiles</t>
+  </si>
+  <si>
+    <t>status=200||userList=(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>/follow/user/(SYS_USER1)(SYS_USER1)/followers/profiles</t>
+  </si>
+  <si>
+    <t>status=404||errorCode=404||errorMessage=User not found</t>
+  </si>
+  <si>
+    <t>/follow/user/(SYS_USER1)/following/profiles</t>
+  </si>
+  <si>
+    <t>/follow/user/(SYS_USER1)(SYS_USER1)/following/profiles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify error status with out passing user in followers time range API </t>
+  </si>
+  <si>
+    <t>/follow/user/(SYS_USER1)/followersByTimeRange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify error status with out passing user in followings time range API </t>
+  </si>
+  <si>
+    <t>/follow/user/(SYS_USER1)/followingsByTimeRange</t>
+  </si>
+  <si>
+    <t>S1_TC_T15</t>
+  </si>
+  <si>
+    <t>S1_TC_T16</t>
+  </si>
+  <si>
+    <t>S1_TC_T17</t>
+  </si>
+  <si>
+    <t>S1_TC_T18</t>
+  </si>
+  <si>
+    <t>S1_TC_T19</t>
+  </si>
+  <si>
+    <t>S1_TC_T20</t>
+  </si>
+  <si>
+    <t>S1_TC_T21</t>
+  </si>
+  <si>
+    <t>S1_TC_T22</t>
+  </si>
+  <si>
+    <t>S1_TC_T23</t>
+  </si>
+  <si>
+    <t>S1_TC_T24</t>
   </si>
 </sst>
 </file>
@@ -567,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L15"/>
+      <selection activeCell="L2" sqref="L2:L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -632,48 +731,52 @@
         <v>12</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>22</v>
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
       </c>
       <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="H2" s="4"/>
       <c r="I2" s="1"/>
-      <c r="J2" t="s">
-        <v>25</v>
+      <c r="J2" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="30">
+    <row r="3" spans="1:12" ht="45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>61</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
-      <c r="J3" t="s">
-        <v>51</v>
+      <c r="J3" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="K3" s="1"/>
     </row>
@@ -682,91 +785,111 @@
         <v>15</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H4"/>
+        <v>26</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="1"/>
       <c r="J4" t="s">
-        <v>17</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="E5" t="s">
         <v>0</v>
       </c>
-      <c r="H5"/>
-      <c r="J5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="45">
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" ht="30">
       <c r="A6" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
         <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
       </c>
-      <c r="H6"/>
-      <c r="J6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" ht="30">
       <c r="A7" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H7"/>
+        <v>26</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="1"/>
       <c r="J7" t="s">
-        <v>35</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="30">
       <c r="A8" t="s">
         <v>40</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
@@ -787,66 +910,62 @@
         <v>41</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9"/>
       <c r="J9" t="s">
-        <v>39</v>
-      </c>
-      <c r="K9" s="1"/>
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="45">
       <c r="A10" t="s">
         <v>47</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="H10"/>
       <c r="J10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="30">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>48</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
         <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="H11"/>
       <c r="J11" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="30">
@@ -854,20 +973,20 @@
         <v>49</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
         <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="H12"/>
       <c r="J12" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30">
@@ -875,13 +994,13 @@
         <v>52</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
         <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>22</v>
@@ -891,7 +1010,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="1"/>
       <c r="J13" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="K13" s="1"/>
     </row>
@@ -900,23 +1019,20 @@
         <v>54</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="C14" t="s">
         <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E14" t="s">
         <v>0</v>
       </c>
       <c r="H14"/>
-      <c r="J14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K14" t="s">
-        <v>58</v>
+      <c r="J14" s="5" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="30">
@@ -924,25 +1040,242 @@
         <v>59</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15"/>
+      <c r="J15" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16"/>
+      <c r="J16" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="30">
+      <c r="A17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17"/>
+      <c r="J17" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="30">
+      <c r="A18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18"/>
+      <c r="J18" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="30">
+      <c r="A19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19"/>
+      <c r="J19" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="45">
+      <c r="A20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20"/>
+      <c r="J20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="30">
+      <c r="A21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21"/>
+      <c r="J21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="30">
+      <c r="A22" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22"/>
+      <c r="J22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="30">
+      <c r="A23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="1"/>
+      <c r="J23" t="s">
+        <v>57</v>
+      </c>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" t="s">
+        <v>0</v>
+      </c>
+      <c r="H24"/>
+      <c r="J24" t="s">
+        <v>17</v>
+      </c>
+      <c r="K24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="30">
+      <c r="A25" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="1"/>
-      <c r="J15" t="s">
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="1"/>
+      <c r="J25" t="s">
         <v>39</v>
       </c>
-      <c r="K15" s="1"/>
+      <c r="K25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Test cases for Groups Changed Test cases descriptions fir search,type ahead, watchlist. Changed input parameters.
</commit_message>
<xml_diff>
--- a/src/test/test-data/FollowTestData.xlsx
+++ b/src/test/test-data/FollowTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="98">
   <si>
     <t>GET</t>
   </si>
@@ -70,15 +70,6 @@
     <t>status=200</t>
   </si>
   <si>
-    <t>Start following a user and verify the follow relationship.</t>
-  </si>
-  <si>
-    <t>Check users whom I am following and verify the response.</t>
-  </si>
-  <si>
-    <t>Check all my followers and verify the response</t>
-  </si>
-  <si>
     <t>1PFOLLOW</t>
   </si>
   <si>
@@ -100,27 +91,18 @@
     <t>S1_TC_T5</t>
   </si>
   <si>
-    <t>Check follow relationship with another user when I am following him and he is not following me</t>
-  </si>
-  <si>
     <t>/follow/user/(SYS_USER1)/relation/(SYS_USER2)</t>
   </si>
   <si>
     <t>/follow/user/(SYS_USER1)/count/following</t>
   </si>
   <si>
-    <t>Check count of users I am following</t>
-  </si>
-  <si>
     <t>status=200||count=1</t>
   </si>
   <si>
     <t>S1_TC_T6</t>
   </si>
   <si>
-    <t>Get and validate the profiles of whom I am following</t>
-  </si>
-  <si>
     <t>/follow/user/(SYS_USER2)/following/(SYS_USER1)</t>
   </si>
   <si>
@@ -130,18 +112,9 @@
     <t>S1_TC_T8</t>
   </si>
   <si>
-    <t>Check count of my followers</t>
-  </si>
-  <si>
     <t>/follow/user/(SYS_USER1)/count/followers</t>
   </si>
   <si>
-    <t>When both are following each other, Stop following a user and verify follow relationship</t>
-  </si>
-  <si>
-    <t>Stop following a user who is not following me</t>
-  </si>
-  <si>
     <t>S1_TC_T9</t>
   </si>
   <si>
@@ -151,24 +124,15 @@
     <t>S1_TC_T11</t>
   </si>
   <si>
-    <t xml:space="preserve">Trying to stop following a user who I am not following </t>
-  </si>
-  <si>
     <t>errorCode=409</t>
   </si>
   <si>
     <t>S1_TC_T12</t>
   </si>
   <si>
-    <t>Try to follaw a user who I am following already</t>
-  </si>
-  <si>
     <t>S1_TC_T13</t>
   </si>
   <si>
-    <t>Get follow relationship for the same user</t>
-  </si>
-  <si>
     <t>/follow/user/(SYS_USER1)/following/(SYS_USER1)</t>
   </si>
   <si>
@@ -178,9 +142,6 @@
     <t>S1_TC_T14</t>
   </si>
   <si>
-    <t>verify follow relationship when the user doesn't follow each other</t>
-  </si>
-  <si>
     <t>/follow/user/(SYS_USER2)/relations</t>
   </si>
   <si>
@@ -190,18 +151,12 @@
     <t>status=200||(SYS_USER1)=IS_NONE</t>
   </si>
   <si>
-    <t>verify follow relationship by passing empty key and test error status</t>
-  </si>
-  <si>
     <t>?id=</t>
   </si>
   <si>
     <t>status=500||errorCode=500||errorMessage=Key may not be empty</t>
   </si>
   <si>
-    <t>verify follow relationship when the user follower of other</t>
-  </si>
-  <si>
     <t>/follow/user/(SYS_USER1)/relations</t>
   </si>
   <si>
@@ -214,9 +169,6 @@
     <t>status=200||(SYS_USER1)=IS_FOLLOWED</t>
   </si>
   <si>
-    <t>Get all followers information</t>
-  </si>
-  <si>
     <t>/follow/user/(SYS_USER1)/followers/profiles</t>
   </si>
   <si>
@@ -235,15 +187,9 @@
     <t>/follow/user/(SYS_USER1)(SYS_USER1)/following/profiles</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify error status with out passing user in followers time range API </t>
-  </si>
-  <si>
     <t>/follow/user/(SYS_USER1)/followersByTimeRange</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify error status with out passing user in followings time range API </t>
-  </si>
-  <si>
     <t>/follow/user/(SYS_USER1)/followingsByTimeRange</t>
   </si>
   <si>
@@ -277,12 +223,6 @@
     <t>S1_TC_T24</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-  <si>
     <t>status=201||followRelationship=IS_FOLLOWER</t>
   </si>
   <si>
@@ -299,13 +239,81 @@
   </si>
   <si>
     <t>status=403||errorMessage=Not allowed</t>
+  </si>
+  <si>
+    <t>Verify that follow relationship when the user doesn't follow each other</t>
+  </si>
+  <si>
+    <t>Verify that follow relationship by passing empty key and test error status</t>
+  </si>
+  <si>
+    <t>Verify that following a user and verify the follow relationship.</t>
+  </si>
+  <si>
+    <t>Verify that follow relationship when the user follower of other</t>
+  </si>
+  <si>
+    <t>Verify that follow a user who I am following already</t>
+  </si>
+  <si>
+    <t>Verify that follow relationship when the user following of other</t>
+  </si>
+  <si>
+    <t>Verify that user is able to get following users information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that user is able to get his followers information </t>
+  </si>
+  <si>
+    <t>Verify that follow relationship with user2 when user1 is following user2 and user2 is not following user1</t>
+  </si>
+  <si>
+    <t>Verify that user is able to get his following users count.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that start following a user who already following to me </t>
+  </si>
+  <si>
+    <t>Verify that error status by passing wring user id to follower profiles api</t>
+  </si>
+  <si>
+    <t>Verify that to get user following profiles information</t>
+  </si>
+  <si>
+    <t>Verify that to get user follower profiles information</t>
+  </si>
+  <si>
+    <t>Verify that error status by passing wring user id to following profiles api</t>
+  </si>
+  <si>
+    <t>Verify that user able to get his followers inforamation based on time, they are following to him</t>
+  </si>
+  <si>
+    <t>Verify that when both the users are following each other, Stop following a user and verify follow relationship</t>
+  </si>
+  <si>
+    <t>Verify that stop following a user who is not following me</t>
+  </si>
+  <si>
+    <t>Verify that stop following a user who I am not following</t>
+  </si>
+  <si>
+    <t>Verify that to get  follow relationship with the same user it self</t>
+  </si>
+  <si>
+    <t>Verify that user is able to test for count of users following me</t>
+  </si>
+  <si>
+    <t>Verify that follow a followed user and verify the follow relationship.</t>
+  </si>
+  <si>
+    <t>Verify that user able to get his following users inforamation based on time,when he following to them</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -364,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -379,6 +387,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,26 +682,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:AO25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="33.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="96.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="29.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="5" width="23.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="52.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="96.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="23.7109375" style="5" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="52" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -733,502 +742,411 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30">
+    <row r="2" spans="1:12" ht="45">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="1"/>
       <c r="J2" s="5" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="K2" s="1"/>
-      <c r="L2" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="3" spans="1:12" ht="45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
       <c r="J3" s="5" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="K3" s="1"/>
-      <c r="L3" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="4" spans="1:12" ht="30">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="4"/>
       <c r="I4" s="1"/>
       <c r="J4" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="K4" s="1"/>
-      <c r="L4" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="E5" t="s">
         <v>0</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="1"/>
       <c r="J5" s="5" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="K5" s="1"/>
-      <c r="L5" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="6" spans="1:12" ht="30">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="1"/>
       <c r="J6" s="5" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="K6" s="1"/>
-      <c r="L6" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="7" spans="1:12" ht="30">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
         <v>21</v>
       </c>
-      <c r="D7" t="s">
-        <v>24</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="4"/>
       <c r="I7" s="1"/>
       <c r="J7" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="K7" s="1"/>
-      <c r="L7" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="8" spans="1:12" ht="30">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
         <v>0</v>
       </c>
-      <c r="F8"/>
-      <c r="G8"/>
       <c r="H8"/>
-      <c r="I8"/>
       <c r="J8" t="s">
         <v>17</v>
       </c>
-      <c r="K8"/>
-      <c r="L8" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="9" spans="1:12" ht="30">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
         <v>0</v>
       </c>
-      <c r="F9"/>
-      <c r="G9"/>
       <c r="H9"/>
-      <c r="I9"/>
       <c r="J9" t="s">
         <v>17</v>
       </c>
-      <c r="K9"/>
-      <c r="L9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="45">
+    </row>
+    <row r="10" spans="1:12" ht="60">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s">
         <v>0</v>
       </c>
-      <c r="F10"/>
-      <c r="G10"/>
       <c r="H10"/>
-      <c r="I10"/>
       <c r="J10" t="s">
-        <v>90</v>
-      </c>
-      <c r="K10"/>
-      <c r="L10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E11" t="s">
         <v>0</v>
       </c>
-      <c r="F11"/>
-      <c r="G11"/>
       <c r="H11"/>
-      <c r="I11"/>
       <c r="J11" t="s">
-        <v>32</v>
-      </c>
-      <c r="K11"/>
-      <c r="L11" t="s">
-        <v>87</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="30">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E12" t="s">
         <v>0</v>
       </c>
-      <c r="F12"/>
-      <c r="G12"/>
       <c r="H12"/>
-      <c r="I12"/>
       <c r="J12" t="s">
         <v>17</v>
       </c>
-      <c r="K12"/>
-      <c r="L12" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="13" spans="1:12" ht="30">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>18</v>
+        <v>85</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="4"/>
       <c r="I13" s="1"/>
       <c r="J13" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="K13" s="1"/>
-      <c r="L13" t="s">
+    </row>
+    <row r="14" spans="1:12" ht="30">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14"/>
+      <c r="J14" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="45">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15"/>
+      <c r="J15" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="30">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" t="s">
-        <v>0</v>
-      </c>
-      <c r="F14"/>
-      <c r="G14"/>
-      <c r="H14"/>
-      <c r="I14"/>
-      <c r="J14" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="K14"/>
-      <c r="L14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="30">
-      <c r="A15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" t="s">
-        <v>0</v>
-      </c>
-      <c r="F15"/>
-      <c r="G15"/>
-      <c r="H15"/>
-      <c r="I15"/>
-      <c r="J15" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="K15"/>
-      <c r="L15" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" t="s">
-        <v>77</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>66</v>
-      </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="E16" t="s">
         <v>0</v>
       </c>
-      <c r="F16"/>
-      <c r="G16"/>
       <c r="H16"/>
-      <c r="I16"/>
       <c r="J16" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="K16"/>
-      <c r="L16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="30">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:41" ht="45">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="E17" t="s">
         <v>0</v>
       </c>
-      <c r="F17"/>
-      <c r="G17"/>
       <c r="H17"/>
-      <c r="I17"/>
       <c r="J17" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="K17"/>
-      <c r="L17" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="30">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:41" ht="45">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="E18" t="s">
         <v>0</v>
       </c>
-      <c r="F18"/>
-      <c r="G18"/>
       <c r="H18"/>
-      <c r="I18"/>
       <c r="J18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K18"/>
-      <c r="L18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="30">
+    </row>
+    <row r="19" spans="1:41" s="6" customFormat="1" ht="45">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="E19" t="s">
         <v>0</v>
@@ -1237,183 +1155,177 @@
       <c r="G19"/>
       <c r="H19"/>
       <c r="I19"/>
-      <c r="J19" s="5" t="s">
+      <c r="J19" t="s">
         <v>17</v>
       </c>
       <c r="K19"/>
-      <c r="L19" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="45">
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+      <c r="Q19"/>
+      <c r="R19"/>
+      <c r="S19"/>
+      <c r="T19"/>
+      <c r="U19"/>
+      <c r="V19"/>
+      <c r="W19"/>
+      <c r="X19"/>
+      <c r="Y19"/>
+      <c r="Z19"/>
+      <c r="AA19"/>
+      <c r="AB19"/>
+      <c r="AC19"/>
+      <c r="AD19"/>
+      <c r="AE19"/>
+      <c r="AF19"/>
+      <c r="AG19"/>
+      <c r="AH19"/>
+      <c r="AI19"/>
+      <c r="AJ19"/>
+      <c r="AK19"/>
+      <c r="AL19"/>
+      <c r="AM19"/>
+      <c r="AN19"/>
+      <c r="AO19"/>
+    </row>
+    <row r="20" spans="1:41" ht="60">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>40</v>
+        <v>91</v>
       </c>
       <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s">
         <v>21</v>
       </c>
-      <c r="D20" t="s">
-        <v>24</v>
-      </c>
       <c r="E20" t="s">
-        <v>23</v>
-      </c>
-      <c r="F20"/>
-      <c r="G20"/>
+        <v>20</v>
+      </c>
       <c r="H20"/>
-      <c r="I20"/>
       <c r="J20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:41" ht="30">
+      <c r="A21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="K20"/>
-      <c r="L20" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="30">
-      <c r="A21" t="s">
-        <v>82</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="C21" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E21" t="s">
-        <v>23</v>
-      </c>
-      <c r="F21"/>
-      <c r="G21"/>
+        <v>20</v>
+      </c>
       <c r="H21"/>
-      <c r="I21"/>
       <c r="J21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:41" ht="30">
+      <c r="A22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="K21"/>
-      <c r="L21" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="30">
-      <c r="A22" t="s">
-        <v>83</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>45</v>
-      </c>
       <c r="C22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D22" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E22" t="s">
-        <v>23</v>
-      </c>
-      <c r="F22"/>
-      <c r="G22"/>
+        <v>20</v>
+      </c>
       <c r="H22"/>
-      <c r="I22"/>
       <c r="J22" t="s">
-        <v>46</v>
-      </c>
-      <c r="K22"/>
-      <c r="L22" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="30">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:41" ht="45">
       <c r="A23" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>50</v>
+        <v>94</v>
       </c>
       <c r="C23" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D23" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="4"/>
       <c r="I23" s="1"/>
       <c r="J23" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="K23" s="1"/>
-      <c r="L23" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
+    </row>
+    <row r="24" spans="1:41" ht="30">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="C24" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E24" t="s">
         <v>0</v>
       </c>
-      <c r="F24"/>
-      <c r="G24"/>
       <c r="H24"/>
-      <c r="I24"/>
       <c r="J24" t="s">
         <v>17</v>
       </c>
       <c r="K24" t="s">
-        <v>52</v>
-      </c>
-      <c r="L24" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="30">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:41" ht="30">
       <c r="A25" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>18</v>
+        <v>96</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D25" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="4"/>
       <c r="I25" s="1"/>
       <c r="J25" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="K25" s="1"/>
-      <c r="L25" t="s">
-        <v>87</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Replaced test case names with jira id's in Follow, Groups and Iam. Fixed validations in Notify. Modified API path in session eviction testcases
</commit_message>
<xml_diff>
--- a/src/test/test-data/FollowTestData.xlsx
+++ b/src/test/test-data/FollowTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="96">
   <si>
     <t>GET</t>
   </si>
@@ -52,21 +52,9 @@
     <t>APIPATH</t>
   </si>
   <si>
-    <t>S1_TC_T1</t>
-  </si>
-  <si>
-    <t>S1_TC_T2</t>
-  </si>
-  <si>
     <t>DEPENDENCYTESTS</t>
   </si>
   <si>
-    <t>S1_TC_T3</t>
-  </si>
-  <si>
-    <t>S1_TC_T4</t>
-  </si>
-  <si>
     <t>status=200</t>
   </si>
   <si>
@@ -88,9 +76,6 @@
     <t>/follow/user/(SYS_USER2)/followers</t>
   </si>
   <si>
-    <t>S1_TC_T5</t>
-  </si>
-  <si>
     <t>/follow/user/(SYS_USER1)/relation/(SYS_USER2)</t>
   </si>
   <si>
@@ -100,48 +85,21 @@
     <t>status=200||count=1</t>
   </si>
   <si>
-    <t>S1_TC_T6</t>
-  </si>
-  <si>
     <t>/follow/user/(SYS_USER2)/following/(SYS_USER1)</t>
   </si>
   <si>
-    <t>S1_TC_T7</t>
-  </si>
-  <si>
-    <t>S1_TC_T8</t>
-  </si>
-  <si>
     <t>/follow/user/(SYS_USER1)/count/followers</t>
   </si>
   <si>
-    <t>S1_TC_T9</t>
-  </si>
-  <si>
-    <t>S1_TC_T10</t>
-  </si>
-  <si>
-    <t>S1_TC_T11</t>
-  </si>
-  <si>
     <t>errorCode=409</t>
   </si>
   <si>
-    <t>S1_TC_T12</t>
-  </si>
-  <si>
-    <t>S1_TC_T13</t>
-  </si>
-  <si>
     <t>/follow/user/(SYS_USER1)/following/(SYS_USER1)</t>
   </si>
   <si>
     <t>count</t>
   </si>
   <si>
-    <t>S1_TC_T14</t>
-  </si>
-  <si>
     <t>/follow/user/(SYS_USER2)/relations</t>
   </si>
   <si>
@@ -193,36 +151,6 @@
     <t>/follow/user/(SYS_USER1)/followingsByTimeRange</t>
   </si>
   <si>
-    <t>S1_TC_T15</t>
-  </si>
-  <si>
-    <t>S1_TC_T16</t>
-  </si>
-  <si>
-    <t>S1_TC_T17</t>
-  </si>
-  <si>
-    <t>S1_TC_T18</t>
-  </si>
-  <si>
-    <t>S1_TC_T19</t>
-  </si>
-  <si>
-    <t>S1_TC_T20</t>
-  </si>
-  <si>
-    <t>S1_TC_T21</t>
-  </si>
-  <si>
-    <t>S1_TC_T22</t>
-  </si>
-  <si>
-    <t>S1_TC_T23</t>
-  </si>
-  <si>
-    <t>S1_TC_T24</t>
-  </si>
-  <si>
     <t>status=201||followRelationship=IS_FOLLOWER</t>
   </si>
   <si>
@@ -301,13 +229,79 @@
     <t>Verify that to get  follow relationship with the same user it self</t>
   </si>
   <si>
-    <t>Verify that user is able to test for count of users following me</t>
-  </si>
-  <si>
-    <t>Verify that follow a followed user and verify the follow relationship.</t>
-  </si>
-  <si>
     <t>Verify that user able to get his following users inforamation based on time,when he following to them</t>
+  </si>
+  <si>
+    <t>OPQA-448</t>
+  </si>
+  <si>
+    <t>OPQA-449</t>
+  </si>
+  <si>
+    <t>OPQA-450</t>
+  </si>
+  <si>
+    <t>OPQA-451</t>
+  </si>
+  <si>
+    <t>OPQA-452</t>
+  </si>
+  <si>
+    <t>OPQA-454</t>
+  </si>
+  <si>
+    <t>OPQA-455</t>
+  </si>
+  <si>
+    <t>OPQA-456</t>
+  </si>
+  <si>
+    <t>OPQA-446</t>
+  </si>
+  <si>
+    <t>OPQA-457</t>
+  </si>
+  <si>
+    <t>OPQA-458</t>
+  </si>
+  <si>
+    <t>OPQA-459</t>
+  </si>
+  <si>
+    <t>OPQA-460</t>
+  </si>
+  <si>
+    <t>OPQA-461</t>
+  </si>
+  <si>
+    <t>OPQA-462</t>
+  </si>
+  <si>
+    <t>OPQA-463</t>
+  </si>
+  <si>
+    <t>Verify that user is able to get his followers count</t>
+  </si>
+  <si>
+    <t>OPQA-447_1</t>
+  </si>
+  <si>
+    <t>OPQA-450_1</t>
+  </si>
+  <si>
+    <t>OPQA-737</t>
+  </si>
+  <si>
+    <t>OPQA-738</t>
+  </si>
+  <si>
+    <t>OPQA-739</t>
+  </si>
+  <si>
+    <t>OPQA-740</t>
+  </si>
+  <si>
+    <t>OPQA-741</t>
   </si>
 </sst>
 </file>
@@ -682,21 +676,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AO25"/>
+  <dimension ref="A1:AO24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L25"/>
+    <sheetView tabSelected="1" topLeftCell="E19" workbookViewId="0">
+      <selection activeCell="L24" sqref="L2:L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="33.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="96.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="23.7109375" style="5" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="18.140625" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="52" bestFit="1" customWidth="1" collapsed="1"/>
@@ -730,7 +724,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>9</v>
@@ -744,591 +738,576 @@
     </row>
     <row r="2" spans="1:12" ht="45">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="1"/>
       <c r="J2" s="5" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="45">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
       <c r="J3" s="5" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="30">
       <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="4"/>
       <c r="I4" s="1"/>
       <c r="J4" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
         <v>0</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="1"/>
       <c r="J5" s="5" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:12" ht="30">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="1"/>
       <c r="J6" s="5" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:12" ht="30">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="4"/>
       <c r="I7" s="1"/>
       <c r="J7" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="30">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
         <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
       </c>
       <c r="E8" t="s">
         <v>0</v>
       </c>
       <c r="H8"/>
       <c r="J8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="30">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>77</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E9" t="s">
         <v>0</v>
       </c>
       <c r="H9"/>
       <c r="J9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="60">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
         <v>0</v>
       </c>
       <c r="H10"/>
       <c r="J10" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E11" t="s">
         <v>0</v>
       </c>
       <c r="H11"/>
       <c r="J11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="30">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" t="s">
-        <v>0</v>
-      </c>
-      <c r="H12"/>
+        <v>23</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="1"/>
       <c r="J12" t="s">
-        <v>17</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:12" ht="30">
       <c r="A13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="1"/>
-      <c r="J13" t="s">
-        <v>71</v>
-      </c>
-      <c r="K13" s="1"/>
-    </row>
-    <row r="14" spans="1:12" ht="30">
+      <c r="E13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13"/>
+      <c r="J13" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="45">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>93</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E14" t="s">
         <v>0</v>
       </c>
       <c r="H14"/>
       <c r="J14" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="45">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="30">
       <c r="A15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
         <v>41</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" t="s">
-        <v>53</v>
       </c>
       <c r="E15" t="s">
         <v>0</v>
       </c>
       <c r="H15"/>
       <c r="J15" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="30">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="45">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E16" t="s">
         <v>0</v>
       </c>
       <c r="H16"/>
       <c r="J16" s="5" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:41" ht="45">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E17" t="s">
         <v>0</v>
       </c>
       <c r="H17"/>
       <c r="J17" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:41" ht="45">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:41" s="6" customFormat="1" ht="45">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="E18" t="s">
         <v>0</v>
       </c>
+      <c r="F18"/>
+      <c r="G18"/>
       <c r="H18"/>
-      <c r="J18" s="5" t="s">
+      <c r="I18"/>
+      <c r="J18" t="s">
+        <v>13</v>
+      </c>
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="O18"/>
+      <c r="P18"/>
+      <c r="Q18"/>
+      <c r="R18"/>
+      <c r="S18"/>
+      <c r="T18"/>
+      <c r="U18"/>
+      <c r="V18"/>
+      <c r="W18"/>
+      <c r="X18"/>
+      <c r="Y18"/>
+      <c r="Z18"/>
+      <c r="AA18"/>
+      <c r="AB18"/>
+      <c r="AC18"/>
+      <c r="AD18"/>
+      <c r="AE18"/>
+      <c r="AF18"/>
+      <c r="AG18"/>
+      <c r="AH18"/>
+      <c r="AI18"/>
+      <c r="AJ18"/>
+      <c r="AK18"/>
+      <c r="AL18"/>
+      <c r="AM18"/>
+      <c r="AN18"/>
+      <c r="AO18"/>
+    </row>
+    <row r="19" spans="1:41" ht="60">
+      <c r="A19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:41" s="6" customFormat="1" ht="45">
-      <c r="A19" t="s">
-        <v>62</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" t="s">
-        <v>58</v>
-      </c>
       <c r="E19" t="s">
-        <v>0</v>
-      </c>
-      <c r="F19"/>
-      <c r="G19"/>
+        <v>16</v>
+      </c>
       <c r="H19"/>
-      <c r="I19"/>
       <c r="J19" t="s">
-        <v>17</v>
-      </c>
-      <c r="K19"/>
-      <c r="L19"/>
-      <c r="M19"/>
-      <c r="N19"/>
-      <c r="O19"/>
-      <c r="P19"/>
-      <c r="Q19"/>
-      <c r="R19"/>
-      <c r="S19"/>
-      <c r="T19"/>
-      <c r="U19"/>
-      <c r="V19"/>
-      <c r="W19"/>
-      <c r="X19"/>
-      <c r="Y19"/>
-      <c r="Z19"/>
-      <c r="AA19"/>
-      <c r="AB19"/>
-      <c r="AC19"/>
-      <c r="AD19"/>
-      <c r="AE19"/>
-      <c r="AF19"/>
-      <c r="AG19"/>
-      <c r="AH19"/>
-      <c r="AI19"/>
-      <c r="AJ19"/>
-      <c r="AK19"/>
-      <c r="AL19"/>
-      <c r="AM19"/>
-      <c r="AN19"/>
-      <c r="AO19"/>
-    </row>
-    <row r="20" spans="1:41" ht="60">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:41" ht="30">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="H20"/>
       <c r="J20" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:41" ht="30">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="C21" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E21" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="H21"/>
       <c r="J21" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:41" ht="30">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:41" ht="45">
       <c r="A22" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" t="s">
-        <v>20</v>
-      </c>
-      <c r="H22"/>
+        <v>26</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="1"/>
       <c r="J22" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:41" ht="45">
+        <v>50</v>
+      </c>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:41" ht="30">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C23" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="E23" t="s">
+        <v>0</v>
+      </c>
+      <c r="H23"/>
       <c r="J23" t="s">
-        <v>74</v>
-      </c>
-      <c r="K23" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="K23" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="24" spans="1:41" ht="30">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>95</v>
+        <v>53</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" t="s">
-        <v>0</v>
-      </c>
-      <c r="H24"/>
+        <v>23</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="1"/>
       <c r="J24" t="s">
-        <v>17</v>
-      </c>
-      <c r="K24" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:41" ht="30">
-      <c r="A25" t="s">
-        <v>68</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C25" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" t="s">
-        <v>29</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="1"/>
-      <c r="J25" t="s">
-        <v>69</v>
-      </c>
-      <c r="K25" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="K24" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A5" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-737"/>
+    <hyperlink ref="A13" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-738"/>
+    <hyperlink ref="A14" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-739"/>
+    <hyperlink ref="A15:A16" r:id="rId4" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-739"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Validation for calculations like addition and subtraction. Modified test cases in to 1PFOLOOW
</commit_message>
<xml_diff>
--- a/src/test/test-data/FollowTestData.xlsx
+++ b/src/test/test-data/FollowTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="106">
   <si>
     <t>GET</t>
   </si>
@@ -82,9 +82,6 @@
     <t>/follow/user/(SYS_USER1)/count/following</t>
   </si>
   <si>
-    <t>status=200||count=1</t>
-  </si>
-  <si>
     <t>/follow/user/(SYS_USER2)/following/(SYS_USER1)</t>
   </si>
   <si>
@@ -286,9 +283,6 @@
     <t>OPQA-447_1</t>
   </si>
   <si>
-    <t>OPQA-450_1</t>
-  </si>
-  <si>
     <t>OPQA-737</t>
   </si>
   <si>
@@ -302,6 +296,42 @@
   </si>
   <si>
     <t>OPQA-741</t>
+  </si>
+  <si>
+    <t>OPQA-446_1</t>
+  </si>
+  <si>
+    <t>status=200||count=eval$(OPQA-446_count)+1</t>
+  </si>
+  <si>
+    <t>OPQA-447</t>
+  </si>
+  <si>
+    <t>Verify that to test following users count increased when user following other user.</t>
+  </si>
+  <si>
+    <t>Verify that to test follower users count increased when user have a new follower.</t>
+  </si>
+  <si>
+    <t>status=200||count=eval$(OPQA-447_count)+1</t>
+  </si>
+  <si>
+    <t>OPQA-446_2</t>
+  </si>
+  <si>
+    <t>Verify that to test following users count decreced when user unfollowing other user.</t>
+  </si>
+  <si>
+    <t>status=200||count=eval$(OPQA-446_1_count)-1</t>
+  </si>
+  <si>
+    <t>Verify that to test follower users count  decreced when user unfollowed him.</t>
+  </si>
+  <si>
+    <t>OPQA-447_2</t>
+  </si>
+  <si>
+    <t>status=200||count=eval$(OPQA-447_1_count)-1</t>
   </si>
 </sst>
 </file>
@@ -676,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AO24"/>
+  <dimension ref="A1:AO27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E19" workbookViewId="0">
-      <selection activeCell="L24" sqref="L2:L24"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -693,7 +723,7 @@
     <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="23.7109375" style="5" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="52" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="54.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -738,140 +768,137 @@
     </row>
     <row r="2" spans="1:12" ht="45">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="1"/>
       <c r="J2" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="45">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
       <c r="J3" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="30">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4"/>
       <c r="J4" t="s">
-        <v>45</v>
-      </c>
-      <c r="K4" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="K4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" t="s">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="G5" s="1"/>
       <c r="H5" s="4"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="5" t="s">
-        <v>35</v>
+      <c r="J5" t="s">
+        <v>44</v>
       </c>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:12" ht="30">
+    <row r="6" spans="1:12" ht="45">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="K6" s="1"/>
+      <c r="H6"/>
+      <c r="I6" t="s">
+        <v>79</v>
+      </c>
+      <c r="J6" t="s">
+        <v>95</v>
+      </c>
+      <c r="K6" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="30">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>55</v>
@@ -880,432 +907,509 @@
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>15</v>
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>0</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="H7" s="4"/>
       <c r="I7" s="1"/>
-      <c r="J7" t="s">
-        <v>25</v>
+      <c r="J7" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="30">
       <c r="A8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
         <v>0</v>
       </c>
-      <c r="H8"/>
-      <c r="J8" t="s">
-        <v>13</v>
-      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:12" ht="30">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" t="s">
-        <v>0</v>
-      </c>
-      <c r="H9"/>
+        <v>17</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="1"/>
       <c r="J9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="60">
+        <v>24</v>
+      </c>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" ht="30">
       <c r="A10" t="s">
         <v>78</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E10" t="s">
         <v>0</v>
       </c>
       <c r="H10"/>
       <c r="J10" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
         <v>0</v>
       </c>
       <c r="H11"/>
       <c r="J11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="30">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="60">
       <c r="A12" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12"/>
       <c r="J12" t="s">
-        <v>47</v>
-      </c>
-      <c r="K12" s="1"/>
+        <v>45</v>
+      </c>
     </row>
     <row r="13" spans="1:12" ht="30">
       <c r="A13" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
         <v>0</v>
       </c>
       <c r="H13"/>
-      <c r="J13" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="45">
+      <c r="J13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="30">
       <c r="A14" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" t="s">
-        <v>0</v>
-      </c>
-      <c r="H14"/>
-      <c r="J14" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="30">
+        <v>22</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="1"/>
+      <c r="J14" t="s">
+        <v>46</v>
+      </c>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" ht="45">
       <c r="A15" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15"/>
+      <c r="J15" t="s">
+        <v>99</v>
+      </c>
+      <c r="K15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="30">
+      <c r="A16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" t="s">
-        <v>0</v>
-      </c>
-      <c r="H15"/>
-      <c r="J15" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="45">
-      <c r="A16" t="s">
-        <v>95</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="C16" t="s">
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E16" t="s">
         <v>0</v>
       </c>
       <c r="H16"/>
       <c r="J16" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:41" ht="45">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E17" t="s">
         <v>0</v>
       </c>
       <c r="H17"/>
       <c r="J17" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:41" ht="30">
+      <c r="A18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18"/>
+      <c r="J18" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:41" ht="45">
+      <c r="A19" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19"/>
+      <c r="J19" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:41" ht="45">
+      <c r="A20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" t="s">
+        <v>0</v>
+      </c>
+      <c r="H20"/>
+      <c r="J20" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:41" s="6" customFormat="1" ht="45">
-      <c r="A18" t="s">
+    <row r="21" spans="1:41" s="6" customFormat="1" ht="45">
+      <c r="A21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21"/>
+      <c r="O21"/>
+      <c r="P21"/>
+      <c r="Q21"/>
+      <c r="R21"/>
+      <c r="S21"/>
+      <c r="T21"/>
+      <c r="U21"/>
+      <c r="V21"/>
+      <c r="W21"/>
+      <c r="X21"/>
+      <c r="Y21"/>
+      <c r="Z21"/>
+      <c r="AA21"/>
+      <c r="AB21"/>
+      <c r="AC21"/>
+      <c r="AD21"/>
+      <c r="AE21"/>
+      <c r="AF21"/>
+      <c r="AG21"/>
+      <c r="AH21"/>
+      <c r="AI21"/>
+      <c r="AJ21"/>
+      <c r="AK21"/>
+      <c r="AL21"/>
+      <c r="AM21"/>
+      <c r="AN21"/>
+      <c r="AO21"/>
+    </row>
+    <row r="22" spans="1:41" ht="60">
+      <c r="A22" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" t="s">
-        <v>0</v>
-      </c>
-      <c r="F18"/>
-      <c r="G18"/>
-      <c r="H18"/>
-      <c r="I18"/>
-      <c r="J18" t="s">
-        <v>13</v>
-      </c>
-      <c r="K18"/>
-      <c r="L18"/>
-      <c r="M18"/>
-      <c r="N18"/>
-      <c r="O18"/>
-      <c r="P18"/>
-      <c r="Q18"/>
-      <c r="R18"/>
-      <c r="S18"/>
-      <c r="T18"/>
-      <c r="U18"/>
-      <c r="V18"/>
-      <c r="W18"/>
-      <c r="X18"/>
-      <c r="Y18"/>
-      <c r="Z18"/>
-      <c r="AA18"/>
-      <c r="AB18"/>
-      <c r="AC18"/>
-      <c r="AD18"/>
-      <c r="AE18"/>
-      <c r="AF18"/>
-      <c r="AG18"/>
-      <c r="AH18"/>
-      <c r="AI18"/>
-      <c r="AJ18"/>
-      <c r="AK18"/>
-      <c r="AL18"/>
-      <c r="AM18"/>
-      <c r="AN18"/>
-      <c r="AO18"/>
-    </row>
-    <row r="19" spans="1:41" ht="60">
-      <c r="A19" t="s">
-        <v>84</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C19" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="B22" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" t="s">
         <v>17</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E22" t="s">
         <v>16</v>
       </c>
-      <c r="H19"/>
-      <c r="J19" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:41" ht="30">
-      <c r="A20" t="s">
-        <v>85</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20"/>
-      <c r="J20" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:41" ht="30">
-      <c r="A21" t="s">
-        <v>86</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21"/>
-      <c r="J21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:41" ht="45">
-      <c r="A22" t="s">
-        <v>87</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="1"/>
+      <c r="H22"/>
       <c r="J22" t="s">
-        <v>50</v>
-      </c>
-      <c r="K22" s="1"/>
-    </row>
-    <row r="23" spans="1:41" ht="30">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:41" ht="45">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="C23" t="s">
         <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E23" t="s">
         <v>0</v>
       </c>
       <c r="H23"/>
+      <c r="I23" t="s">
+        <v>94</v>
+      </c>
       <c r="J23" t="s">
-        <v>13</v>
-      </c>
-      <c r="K23" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:41" ht="30">
       <c r="A24" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="C24" t="s">
         <v>14</v>
       </c>
       <c r="D24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24"/>
+      <c r="J24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:41" ht="45">
+      <c r="A25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E25" t="s">
+        <v>0</v>
+      </c>
+      <c r="H25"/>
+      <c r="J25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:41" ht="30">
+      <c r="A26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26"/>
+      <c r="J26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:41" ht="45">
+      <c r="A27" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="1"/>
-      <c r="J24" t="s">
-        <v>45</v>
-      </c>
-      <c r="K24" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="1"/>
+      <c r="J27" t="s">
+        <v>49</v>
+      </c>
+      <c r="K27" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A5" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-737"/>
-    <hyperlink ref="A13" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-738"/>
-    <hyperlink ref="A14" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-739"/>
-    <hyperlink ref="A15:A16" r:id="rId4" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-739"/>
+    <hyperlink ref="A7" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-737"/>
+    <hyperlink ref="A16" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-738"/>
+    <hyperlink ref="A17" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-739"/>
+    <hyperlink ref="A18:A19" r:id="rId4" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-739"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>